<commit_message>
Made three tables and fixed Figure 2
</commit_message>
<xml_diff>
--- a/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
+++ b/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$8</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">Cruise </t>
   </si>
@@ -36,15 +36,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>In-situ</t>
-  </si>
-  <si>
-    <t>Nutrients</t>
-  </si>
-  <si>
-    <t>HPLC</t>
-  </si>
-  <si>
     <t>SE-08-02</t>
   </si>
   <si>
@@ -57,18 +48,12 @@
     <t>158°00'W</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>km [nmi]</t>
   </si>
   <si>
     <t>Transect length</t>
   </si>
   <si>
-    <t>Data Collected</t>
-  </si>
-  <si>
     <t>26 March-3 April 2008</t>
   </si>
   <si>
@@ -84,20 +69,41 @@
     <t>1111 [600]</t>
   </si>
   <si>
-    <t>Fluorescence</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>Table 1.Oscar Elton Sette (SE) shipboard survey information for data used in this study</t>
+    <t>Frontal Positions</t>
+  </si>
+  <si>
+    <t>STF</t>
+  </si>
+  <si>
+    <t>TZCF</t>
+  </si>
+  <si>
+    <t>32°15'-32°45'N</t>
+  </si>
+  <si>
+    <t>31°15'-32°15'N</t>
+  </si>
+  <si>
+    <t>34°15'-35°45'N</t>
+  </si>
+  <si>
+    <t>35°00'-36°00'N</t>
+  </si>
+  <si>
+    <t>33°15'-34°15'N</t>
+  </si>
+  <si>
+    <t>Table 1. Oscar Elton Sette (SE) shipboard survey information for data used in this study with geographic boxes used to define frontal areas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,12 +112,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -138,6 +138,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,83 +247,104 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -322,6 +354,12 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -331,6 +369,12 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -671,157 +715,148 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="9.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="7" width="11.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="C7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="F7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F3:I3"/>
+  <mergeCells count="2">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A1:G2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Work on possible wind figures and figure captions added
</commit_message>
<xml_diff>
--- a/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
+++ b/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
@@ -247,8 +247,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -292,12 +296,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,6 +335,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -344,7 +348,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -360,6 +364,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -375,6 +381,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,7 +715,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -757,92 +765,92 @@
       <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final figures for Revision Submission
</commit_message>
<xml_diff>
--- a/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
+++ b/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
@@ -158,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,17 +176,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -195,57 +184,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -284,20 +222,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,46 +234,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -715,7 +626,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:G7"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -730,127 +641,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned figures and tables based on Editor's comments for resubmission #3
</commit_message>
<xml_diff>
--- a/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
+++ b/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="2620" yWindow="4960" windowWidth="35120" windowHeight="22940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">Cruise </t>
   </si>
@@ -30,12 +30,6 @@
     <t>Dates</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>SE-08-02</t>
   </si>
   <si>
@@ -45,30 +39,15 @@
     <t>SE-11-02</t>
   </si>
   <si>
-    <t>158°00'W</t>
-  </si>
-  <si>
-    <t>km [nmi]</t>
-  </si>
-  <si>
-    <t>Transect length</t>
-  </si>
-  <si>
     <t>26 March-3 April 2008</t>
   </si>
   <si>
-    <t>26°00'-36°00'N</t>
-  </si>
-  <si>
     <t>18 March-23 March 2009</t>
   </si>
   <si>
     <t>10 March-23 March 2011</t>
   </si>
   <si>
-    <t>1111 [600]</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -96,7 +75,7 @@
     <t>33°15'-34°15'N</t>
   </si>
   <si>
-    <t>Table 1. Oscar Elton Sette (SE) shipboard survey information for data used in this study with geographic boxes used to define frontal areas</t>
+    <t>Table 1. Oscar Elton Sette (SE) shipboard survey information for data used in this study with geographic boxes used to define frontal areas. All transects were from 26°-36°N along 158°W. Frontal positions were determined using CTD profile data.</t>
   </si>
 </sst>
 </file>
@@ -222,29 +201,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -626,7 +593,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -634,145 +601,104 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="7" width="11.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="10"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>22</v>
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>23</v>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Cleanup of figures, tables, and data in prep for 3rd revision
</commit_message>
<xml_diff>
--- a/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
+++ b/Table 1 - Shipboard surveys/Table 1 - Howell-et-al-Revise.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="4960" windowWidth="35120" windowHeight="22940" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="1200" windowWidth="35120" windowHeight="22940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -601,7 +601,7 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="7" width="11.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>

</xml_diff>